<commit_message>
code added with all expiry dates
</commit_message>
<xml_diff>
--- a/option_chain - Copy.xlsx
+++ b/option_chain - Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cb4cecaa05735e09/Desktop/bipinmsit/tradetools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="842" documentId="11_F25DC773A252ABDACC1048C589D870065ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D56EAB5D-0C5C-4B88-8191-38C3E981A443}"/>
+  <xr:revisionPtr revIDLastSave="2675" documentId="11_F25DC773A252ABDACC1048C589D870065ADE58E8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A344821-C1F9-44DC-AEAF-BA4331DA4909}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Call_LTP</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Index</t>
   </si>
   <si>
-    <t>Expiry</t>
-  </si>
-  <si>
     <t>Spot</t>
   </si>
   <si>
@@ -70,6 +67,15 @@
   </si>
   <si>
     <t>No_of_Strike</t>
+  </si>
+  <si>
+    <t>BANKNIFTY</t>
+  </si>
+  <si>
+    <t>FINNIFTY</t>
+  </si>
+  <si>
+    <t>MIDCPNIFTY</t>
   </si>
 </sst>
 </file>
@@ -93,7 +99,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -112,12 +118,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -131,7 +131,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -148,20 +148,14 @@
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -448,35 +442,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S150"/>
+  <dimension ref="A1:R150"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O6" sqref="O6"/>
+      <selection pane="bottomLeft" activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.08984375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.26953125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.1796875" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="7.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.26953125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.26953125" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.6328125" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="3" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3" style="2" customWidth="1"/>
-    <col min="18" max="16384" width="5" style="2"/>
+    <col min="14" max="14" width="10.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="8.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -510,641 +504,500 @@
         <v>10</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>247.45</v>
+        <v>177.15</v>
       </c>
       <c r="C2" s="2">
-        <v>11485</v>
+        <v>186682</v>
       </c>
       <c r="D2" s="2">
-        <v>-906</v>
+        <v>52314</v>
       </c>
       <c r="E2" s="3">
-        <v>21950</v>
+        <v>22300</v>
       </c>
       <c r="F2" s="2">
-        <v>26291</v>
+        <v>375542</v>
       </c>
       <c r="G2" s="2">
-        <v>91758</v>
+        <v>417234</v>
       </c>
       <c r="H2" s="2">
-        <v>11.3</v>
+        <v>1.45</v>
       </c>
       <c r="I2" s="2">
-        <f>IF(G2&gt;0, G2/C2, "")</f>
-        <v>7.9893774488463212</v>
+        <f>IF(G2&gt;0, ROUND(G2/C2,3), "")</f>
+        <v>2.2349999999999999</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="K2" s="2">
         <f>SUM(D2:D200)</f>
-        <v>199143</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="M2" s="10">
+        <v>1236416</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="7">
         <v>45379</v>
       </c>
-      <c r="N2" s="9">
+      <c r="N2" s="8">
+        <v>45385</v>
+      </c>
+      <c r="O2" s="8">
+        <v>45384</v>
+      </c>
+      <c r="P2" s="8">
+        <v>45383</v>
+      </c>
+      <c r="Q2" s="6">
         <v>3</v>
       </c>
-      <c r="O2" s="9">
-        <v>22175.599999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="R2" s="6">
+        <v>22456.15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>203.45</v>
+        <v>125</v>
       </c>
       <c r="C3" s="2">
-        <v>104249</v>
+        <v>187938</v>
       </c>
       <c r="D3" s="2">
-        <v>-9623</v>
+        <v>73115</v>
       </c>
       <c r="E3" s="3">
-        <v>22000</v>
+        <v>22350</v>
       </c>
       <c r="F3" s="2">
-        <v>86474</v>
+        <v>272834</v>
       </c>
       <c r="G3" s="2">
-        <v>308246</v>
+        <v>276304</v>
       </c>
       <c r="H3" s="2">
-        <v>17.05</v>
+        <v>2.35</v>
       </c>
       <c r="I3" s="2">
-        <f t="shared" ref="I3:I66" si="0">IF(G3&gt;0, G3/C3, "")</f>
-        <v>2.9568245258947328</v>
+        <f t="shared" ref="I3:I66" si="0">IF(G3&gt;0, ROUND(G3/C3,3), "")</f>
+        <v>1.47</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="K3" s="2">
         <f>SUM(F2:F200)</f>
-        <v>573074</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+        <v>2008729</v>
+      </c>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>161.5</v>
+        <v>78.25</v>
       </c>
       <c r="C4" s="2">
-        <v>50461</v>
+        <v>266382</v>
       </c>
       <c r="D4" s="2">
-        <v>-9756</v>
+        <v>80579</v>
       </c>
       <c r="E4" s="3">
-        <v>22050</v>
+        <v>22400</v>
       </c>
       <c r="F4" s="2">
-        <v>59273</v>
+        <v>431853</v>
       </c>
       <c r="G4" s="2">
-        <v>117686</v>
+        <v>447388</v>
       </c>
       <c r="H4" s="2">
-        <v>24.8</v>
+        <v>5.4</v>
       </c>
       <c r="I4" s="2">
         <f t="shared" si="0"/>
-        <v>2.3322169596321913</v>
+        <v>1.679</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="K4" s="4">
         <f>ROUND(SUM(G2:G200)/SUM(C2:C200), 3)</f>
-        <v>1.0229999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+        <v>0.91100000000000003</v>
+      </c>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>122.65</v>
+        <v>36.950000000000003</v>
       </c>
       <c r="C5" s="2">
-        <v>166298</v>
+        <v>249083</v>
       </c>
       <c r="D5" s="2">
-        <v>20753</v>
+        <v>132109</v>
       </c>
       <c r="E5" s="3">
-        <v>22100</v>
+        <v>22450</v>
       </c>
       <c r="F5" s="2">
-        <v>169831</v>
+        <v>352377</v>
       </c>
       <c r="G5" s="2">
-        <v>305517</v>
+        <v>353748</v>
       </c>
       <c r="H5" s="2">
-        <v>36.049999999999997</v>
+        <v>12.4</v>
       </c>
       <c r="I5" s="2">
         <f t="shared" si="0"/>
-        <v>1.8371658107734308</v>
+        <v>1.42</v>
       </c>
       <c r="J5" s="5">
-        <v>0.5400462962962963</v>
+        <v>0.61675925925925923</v>
       </c>
       <c r="K5" s="2">
-        <v>2.9820000000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+        <v>1.129</v>
+      </c>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>88.9</v>
+        <v>6.3</v>
       </c>
       <c r="C6" s="2">
-        <v>109093</v>
+        <v>542335</v>
       </c>
       <c r="D6" s="2">
-        <v>49349</v>
+        <v>285274</v>
       </c>
       <c r="E6" s="3">
-        <v>22150</v>
+        <v>22500</v>
       </c>
       <c r="F6" s="2">
-        <v>102497</v>
+        <v>438579</v>
       </c>
       <c r="G6" s="2">
-        <v>136144</v>
+        <v>460240</v>
       </c>
       <c r="H6" s="2">
-        <v>52.35</v>
+        <v>32.9</v>
       </c>
       <c r="I6" s="2">
         <f t="shared" si="0"/>
-        <v>1.2479627473806751</v>
+        <v>0.84899999999999998</v>
       </c>
       <c r="J6" s="5">
-        <v>0.54144675925925922</v>
+        <v>0.61750000000000005</v>
       </c>
       <c r="K6" s="2">
-        <v>3.0070000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+        <v>1.141</v>
+      </c>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>5</v>
       </c>
       <c r="B7" s="2">
-        <v>60.25</v>
+        <v>1.05</v>
       </c>
       <c r="C7" s="2">
-        <v>182039</v>
+        <v>377938</v>
       </c>
       <c r="D7" s="2">
-        <v>50392</v>
+        <v>311825</v>
       </c>
       <c r="E7" s="3">
-        <v>22200</v>
+        <v>22550</v>
       </c>
       <c r="F7" s="2">
-        <v>88017</v>
+        <v>103427</v>
       </c>
       <c r="G7" s="2">
-        <v>134547</v>
+        <v>104149</v>
       </c>
       <c r="H7" s="2">
-        <v>74.099999999999994</v>
+        <v>77.3</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" si="0"/>
-        <v>0.73911084987282949</v>
+        <v>0.27600000000000002</v>
       </c>
       <c r="J7" s="5">
-        <v>0.54340277777777779</v>
+        <v>0.61908564814814815</v>
       </c>
       <c r="K7" s="2">
-        <v>3.032</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+        <v>1.6020000000000001</v>
+      </c>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="8"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>37.299999999999997</v>
+        <v>0.5</v>
       </c>
       <c r="C8" s="2">
-        <v>85315</v>
+        <v>490189</v>
       </c>
       <c r="D8" s="2">
-        <v>29019</v>
+        <v>301200</v>
       </c>
       <c r="E8" s="3">
-        <v>22250</v>
+        <v>22600</v>
       </c>
       <c r="F8" s="2">
-        <v>14130</v>
+        <v>34117</v>
       </c>
       <c r="G8" s="2">
-        <v>23780</v>
+        <v>37786</v>
       </c>
       <c r="H8" s="2">
-        <v>101.35</v>
+        <v>127.05</v>
       </c>
       <c r="I8" s="2">
         <f t="shared" si="0"/>
-        <v>0.27873175877629958</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="J8" s="5">
-        <v>0.54479166666666667</v>
+        <v>0.61990740740740746</v>
       </c>
       <c r="K8" s="2">
-        <v>3.032</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A9" s="2">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2">
-        <v>21.5</v>
-      </c>
-      <c r="C9" s="2">
-        <v>127580</v>
-      </c>
-      <c r="D9" s="2">
-        <v>-368</v>
-      </c>
-      <c r="E9" s="3">
-        <v>22300</v>
-      </c>
-      <c r="F9" s="2">
-        <v>22701</v>
-      </c>
-      <c r="G9" s="2">
-        <v>52079</v>
-      </c>
-      <c r="H9" s="2">
-        <v>135.75</v>
-      </c>
-      <c r="I9" s="2">
-        <f t="shared" si="0"/>
-        <v>0.40820661545696818</v>
+        <v>1.613</v>
+      </c>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="I9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="J9" s="5">
-        <v>0.5461921296296296</v>
+        <v>0.62177083333333327</v>
       </c>
       <c r="K9" s="2">
-        <v>2.9729999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A10" s="2">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2">
-        <v>11.45</v>
-      </c>
-      <c r="C10" s="2">
-        <v>88508</v>
-      </c>
-      <c r="D10" s="2">
-        <v>14325</v>
-      </c>
-      <c r="E10" s="3">
-        <v>22350</v>
-      </c>
-      <c r="F10" s="2">
-        <v>2493</v>
-      </c>
-      <c r="G10" s="2">
-        <v>6584</v>
-      </c>
-      <c r="H10" s="2">
-        <v>175</v>
-      </c>
-      <c r="I10" s="2">
-        <f t="shared" si="0"/>
-        <v>7.4388755818683053E-2</v>
+        <v>1.163</v>
+      </c>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="I10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="J10" s="5">
-        <v>0.54759259259259252</v>
+        <v>0.62180555555555561</v>
       </c>
       <c r="K10" s="2">
-        <v>3.0609999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A11" s="2">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2">
-        <v>5.5</v>
-      </c>
-      <c r="C11" s="2">
-        <v>165840</v>
-      </c>
-      <c r="D11" s="2">
-        <v>42164</v>
-      </c>
-      <c r="E11" s="3">
-        <v>22400</v>
-      </c>
-      <c r="F11" s="2">
-        <v>1194</v>
-      </c>
-      <c r="G11" s="2">
-        <v>15745</v>
-      </c>
-      <c r="H11" s="2">
-        <v>219.5</v>
-      </c>
-      <c r="I11" s="2">
-        <f t="shared" si="0"/>
-        <v>9.4940906898215147E-2</v>
+        <v>1.613</v>
+      </c>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="I11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="J11" s="5">
-        <v>0.54899305555555555</v>
+        <v>0.62192129629629633</v>
       </c>
       <c r="K11" s="2">
-        <v>3.0459999999999998</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A12" s="2">
-        <v>10</v>
-      </c>
-      <c r="B12" s="2">
-        <v>2.6</v>
-      </c>
-      <c r="C12" s="2">
-        <v>75454</v>
-      </c>
-      <c r="D12" s="2">
-        <v>13794</v>
-      </c>
-      <c r="E12" s="3">
-        <v>22450</v>
-      </c>
-      <c r="F12" s="2">
-        <v>173</v>
-      </c>
-      <c r="G12" s="2">
-        <v>1270</v>
-      </c>
-      <c r="H12" s="2">
-        <v>265.89999999999998</v>
-      </c>
-      <c r="I12" s="2">
-        <f t="shared" si="0"/>
-        <v>1.6831446974315475E-2</v>
+        <v>1.163</v>
+      </c>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="I12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="J12" s="5">
-        <v>0.55040509259259263</v>
+        <v>0.62284722222222222</v>
       </c>
       <c r="K12" s="2">
-        <v>3.1379999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+        <v>1.625</v>
+      </c>
+      <c r="M12" s="8"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="I13" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J13" s="5">
-        <v>0.55180555555555555</v>
-      </c>
-      <c r="K13" s="2">
-        <v>2.964</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="M13" s="8"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="I14" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J14" s="5">
-        <v>0.55320601851851847</v>
-      </c>
-      <c r="K14" s="2">
-        <v>2.964</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="M14" s="8"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="I15" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J15" s="5">
-        <v>0.55459490740740736</v>
-      </c>
-      <c r="K15" s="2">
-        <v>2.9510000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="M15" s="8"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="I16" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J16" s="5">
-        <v>0.55599537037037039</v>
-      </c>
-      <c r="K16" s="2">
-        <v>2.964</v>
-      </c>
-    </row>
-    <row r="17" spans="9:11" x14ac:dyDescent="0.35">
+      <c r="M16" s="8"/>
+    </row>
+    <row r="17" spans="9:13" x14ac:dyDescent="0.35">
       <c r="I17" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J17" s="5">
-        <v>0.55739583333333331</v>
-      </c>
-      <c r="K17" s="2">
-        <v>2.9550000000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="9:11" x14ac:dyDescent="0.35">
+      <c r="M17" s="8"/>
+    </row>
+    <row r="18" spans="9:13" x14ac:dyDescent="0.35">
       <c r="I18" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J18" s="5">
-        <v>0.55879629629629635</v>
-      </c>
-      <c r="K18" s="2">
-        <v>2.948</v>
-      </c>
-    </row>
-    <row r="19" spans="9:11" x14ac:dyDescent="0.35">
+      <c r="M18" s="8"/>
+    </row>
+    <row r="19" spans="9:13" x14ac:dyDescent="0.35">
       <c r="I19" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J19" s="5">
-        <v>0.56019675925925927</v>
-      </c>
-      <c r="K19" s="2">
-        <v>2.8940000000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="9:11" x14ac:dyDescent="0.35">
+      <c r="M19" s="8"/>
+    </row>
+    <row r="20" spans="9:13" x14ac:dyDescent="0.35">
       <c r="I20" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J20" s="5">
-        <v>0.56160879629629623</v>
-      </c>
-      <c r="K20" s="2">
-        <v>2.9140000000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="9:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="9:13" x14ac:dyDescent="0.35">
       <c r="I21" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J21" s="5">
-        <v>0.56304398148148149</v>
-      </c>
-      <c r="K21" s="2">
-        <v>2.99</v>
-      </c>
-    </row>
-    <row r="22" spans="9:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="9:13" x14ac:dyDescent="0.35">
       <c r="I22" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J22" s="5">
-        <v>0.56445601851851845</v>
-      </c>
-      <c r="K22" s="2">
-        <v>3.0579999999999998</v>
-      </c>
-    </row>
-    <row r="23" spans="9:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="9:13" x14ac:dyDescent="0.35">
       <c r="I23" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J23" s="5">
-        <v>0.56586805555555553</v>
-      </c>
-      <c r="K23" s="2">
-        <v>3.0640000000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="9:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="9:13" x14ac:dyDescent="0.35">
       <c r="I24" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J24" s="5">
-        <v>0.5672800925925926</v>
-      </c>
-      <c r="K24" s="2">
-        <v>3.0680000000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="9:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="9:13" x14ac:dyDescent="0.35">
       <c r="I25" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J25" s="5">
-        <v>0.56869212962962956</v>
-      </c>
-      <c r="K25" s="2">
-        <v>3.1080000000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="9:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="9:13" x14ac:dyDescent="0.35">
       <c r="I26" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J26" s="5">
-        <v>0.57010416666666663</v>
-      </c>
-      <c r="K26" s="2">
-        <v>3.137</v>
-      </c>
-    </row>
-    <row r="27" spans="9:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="9:13" x14ac:dyDescent="0.35">
       <c r="I27" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J27" s="5">
-        <v>0.57151620370370371</v>
-      </c>
-      <c r="K27" s="2">
-        <v>3.1659999999999999</v>
-      </c>
-    </row>
-    <row r="28" spans="9:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="9:13" x14ac:dyDescent="0.35">
       <c r="I28" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J28" s="5">
-        <v>0.57297453703703705</v>
-      </c>
-      <c r="K28" s="2">
-        <v>2.8780000000000001</v>
-      </c>
-    </row>
-    <row r="29" spans="9:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="9:13" x14ac:dyDescent="0.35">
       <c r="I29" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="30" spans="9:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="9:13" x14ac:dyDescent="0.35">
       <c r="I30" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="31" spans="9:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="9:13" x14ac:dyDescent="0.35">
       <c r="I31" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
-    <row r="32" spans="9:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="9:13" x14ac:dyDescent="0.35">
       <c r="I32" s="2" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1356,7 +1209,7 @@
     </row>
     <row r="67" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I67" s="2" t="str">
-        <f t="shared" ref="I67:I130" si="1">IF(G67&gt;0, G67/C67, "")</f>
+        <f t="shared" ref="I67:I130" si="1">IF(G67&gt;0, ROUND(G67/C67,3), "")</f>
         <v/>
       </c>
     </row>
@@ -1740,7 +1593,7 @@
     </row>
     <row r="131" spans="9:9" x14ac:dyDescent="0.35">
       <c r="I131" s="2" t="str">
-        <f t="shared" ref="I131:I150" si="2">IF(G131&gt;0, G131/C131, "")</f>
+        <f t="shared" ref="I131:I150" si="2">IF(G131&gt;0, ROUND(G131/C131,3), "")</f>
         <v/>
       </c>
     </row>
@@ -1859,15 +1712,27 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2" xr:uid="{96B84952-593E-4414-97B0-5B64851D6666}">
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7:K10 J6 L6 M7:M10 J5 L3:L4 Q2" xr:uid="{4CBC4F7A-CAE0-4273-9B44-B686111ECF83}">
+      <formula1>"""3,5,10,15,20"""</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J10 L6:L10 L3:L4" xr:uid="{638F3690-EE2A-454A-9984-B221A0E4CF0F}">
+      <formula1>"""NIFTY,BANKNIFTY,FINNIFTY,MIDCPNIFTY,SENSEX"""</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2" xr:uid="{1CBDF931-DD4D-4825-A66A-4FEF531E64FA}">
       <formula1>"""28-Mar-2024,04-Apr-2024,10-Apr-2024,18-Apr-2024,25-Apr-2024,02-May-2024,30-May-2024,27-Jun-2024,26-Sep-2024,26-Dec-2024,26-Jun-2025,24-Dec-2025,25-Jun-2026,31-Dec-2026,24-Jun-2027,30-Dec-2027,29-Jun-2028,28-Dec-2028"""</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2 K7:K10 M8:M10 L3:L4 J5:J6" xr:uid="{4CBC4F7A-CAE0-4273-9B44-B686111ECF83}">
-      <formula1>"""3,5,10,15,20"""</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2" xr:uid="{773D6187-3C21-4CFB-986C-BAAE6CF57711}">
+      <formula1>"""03-Apr-2024,10-Apr-2024,16-Apr-2024,24-Apr-2024,30-Apr-2024,29-May-2024,26-Jun-2024,25-Sep-2024,24-Dec-2024,26-Mar-2025"""</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J10 L2:L4 L8:L10" xr:uid="{638F3690-EE2A-454A-9984-B221A0E4CF0F}">
-      <formula1>"""NIFTY,BANKNIFTY,FINNIFTY,MIDCPNIFTY,SENSEX"""</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2" xr:uid="{478B916E-0B19-492A-8B86-5940E735B419}">
+      <formula1>"""02-Apr-2024,09-Apr-2024,16-Apr-2024,23-Apr-2024,30-Apr-2024,28-May-2024,25-Jun-2024"""</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2" xr:uid="{4DA76A91-6DD4-4492-8D94-9A9CA490D58C}">
+      <formula1>"""NIFTY,BANKNIFTY,FINNIFTY,MIDCPNIFTY"""</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2" xr:uid="{C95600A7-9701-477B-B112-B3EEF3FCBA36}">
+      <formula1>""""""</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>